<commit_message>
atualizacoes dos scripts do nanda
</commit_message>
<xml_diff>
--- a/Documentos/nanda/dominio04/Caracteristica_Dominio04.xlsx
+++ b/Documentos/nanda/dominio04/Caracteristica_Dominio04.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="19440" windowHeight="7995"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
     <sheet name="Plan2" sheetId="2" r:id="rId2"/>
     <sheet name="Plan3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="114210"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1284" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1356" uniqueCount="330">
   <si>
     <t xml:space="preserve">Aumento do absenteísmo (p. ex., no trabalho ou na escola) </t>
   </si>
@@ -952,13 +952,67 @@
   </si>
   <si>
     <t xml:space="preserve">Membros da família pedem ajuda para a manutenção da casa </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Andar de um lado para o outro </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comportamentos como se procurasse alguma coisa </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comportamentos de examinar atentamente </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entrar em local proibido </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hiperatividade </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Incapacidade de localizar marcos significativos em um ambiente familiar </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Locomoção ao acaso </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Locomoção inquieta </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Locomoção persistente em busca de alguma coisa </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Locomoção por espaços não autorizados ou privados </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Locomoção que não pode ser facilmente dissuadida </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Locomoção resultando em abandono não intencional de um local </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Longos períodos de locomoção sem destino aparente </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Movimento contínuo de um lugar a outro </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Movimento frequente de um lugar a outro </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perder-se </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Períodos de locomoção intercalados com períodos de não locomoção (p. ex., sentar, levantar-se, dormir) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Repetir movimentos do cuidador </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -995,18 +1049,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1044,7 +1093,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1078,7 +1127,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1113,10 +1161,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1289,17 +1336,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E321"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E339"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A313" workbookViewId="0">
+      <selection activeCell="D321" sqref="D321"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="4" max="4" width="161.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -1316,7 +1365,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -1333,7 +1382,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -1350,7 +1399,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1367,7 +1416,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1384,7 +1433,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1401,7 +1450,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -1418,7 +1467,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -1435,7 +1484,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -1452,7 +1501,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -1469,7 +1518,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -1486,7 +1535,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1503,7 +1552,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -1520,7 +1569,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -1537,7 +1586,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1554,7 +1603,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1571,7 +1620,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1588,7 +1637,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1605,7 +1654,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -1622,7 +1671,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -1639,7 +1688,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -1656,7 +1705,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>16</v>
       </c>
@@ -1673,7 +1722,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>16</v>
       </c>
@@ -1690,7 +1739,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>16</v>
       </c>
@@ -1707,7 +1756,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>16</v>
       </c>
@@ -1724,7 +1773,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>16</v>
       </c>
@@ -1741,7 +1790,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>16</v>
       </c>
@@ -1758,7 +1807,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>16</v>
       </c>
@@ -1775,7 +1824,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>16</v>
       </c>
@@ -1792,7 +1841,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
         <v>16</v>
       </c>
@@ -1809,7 +1858,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -1826,7 +1875,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5">
       <c r="A32" t="s">
         <v>16</v>
       </c>
@@ -1843,7 +1892,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5">
       <c r="A33" t="s">
         <v>16</v>
       </c>
@@ -1860,7 +1909,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5">
       <c r="A34" t="s">
         <v>16</v>
       </c>
@@ -1877,7 +1926,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5">
       <c r="A35" t="s">
         <v>16</v>
       </c>
@@ -1894,7 +1943,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5">
       <c r="A36" t="s">
         <v>16</v>
       </c>
@@ -1911,7 +1960,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5">
       <c r="A37" t="s">
         <v>16</v>
       </c>
@@ -1928,7 +1977,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5">
       <c r="A38" t="s">
         <v>16</v>
       </c>
@@ -1945,7 +1994,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5">
       <c r="A39" t="s">
         <v>16</v>
       </c>
@@ -1962,7 +2011,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5">
       <c r="A40" t="s">
         <v>16</v>
       </c>
@@ -1979,7 +2028,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5">
       <c r="A41" t="s">
         <v>16</v>
       </c>
@@ -1996,7 +2045,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5">
       <c r="A42" t="s">
         <v>16</v>
       </c>
@@ -2013,7 +2062,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5">
       <c r="A43" t="s">
         <v>16</v>
       </c>
@@ -2030,7 +2079,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5">
       <c r="A44" t="s">
         <v>16</v>
       </c>
@@ -2047,7 +2096,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5">
       <c r="A45" t="s">
         <v>16</v>
       </c>
@@ -2064,7 +2113,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5">
       <c r="A46" t="s">
         <v>16</v>
       </c>
@@ -2081,7 +2130,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5">
       <c r="A47" t="s">
         <v>16</v>
       </c>
@@ -2098,7 +2147,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5">
       <c r="A48" t="s">
         <v>16</v>
       </c>
@@ -2115,7 +2164,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5">
       <c r="A49" t="s">
         <v>16</v>
       </c>
@@ -2132,7 +2181,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5">
       <c r="A50" t="s">
         <v>16</v>
       </c>
@@ -2149,7 +2198,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5">
       <c r="A51" t="s">
         <v>16</v>
       </c>
@@ -2166,7 +2215,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5">
       <c r="A52" t="s">
         <v>16</v>
       </c>
@@ -2183,7 +2232,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5">
       <c r="A53" t="s">
         <v>16</v>
       </c>
@@ -2200,7 +2249,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5">
       <c r="A54" t="s">
         <v>16</v>
       </c>
@@ -2217,7 +2266,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5">
       <c r="A55" t="s">
         <v>16</v>
       </c>
@@ -2234,7 +2283,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5">
       <c r="A56" t="s">
         <v>16</v>
       </c>
@@ -2251,7 +2300,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5">
       <c r="A57" t="s">
         <v>16</v>
       </c>
@@ -2268,7 +2317,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5">
       <c r="A58" t="s">
         <v>16</v>
       </c>
@@ -2285,7 +2334,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5">
       <c r="A59" t="s">
         <v>16</v>
       </c>
@@ -2302,7 +2351,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5">
       <c r="A60" t="s">
         <v>16</v>
       </c>
@@ -2319,7 +2368,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5">
       <c r="A61" t="s">
         <v>16</v>
       </c>
@@ -2336,7 +2385,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5">
       <c r="A62" t="s">
         <v>16</v>
       </c>
@@ -2353,7 +2402,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5">
       <c r="A63" t="s">
         <v>16</v>
       </c>
@@ -2370,7 +2419,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5">
       <c r="A64" t="s">
         <v>16</v>
       </c>
@@ -2387,7 +2436,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5">
       <c r="A65" t="s">
         <v>16</v>
       </c>
@@ -2404,7 +2453,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5">
       <c r="A66" t="s">
         <v>16</v>
       </c>
@@ -2421,7 +2470,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5">
       <c r="A67" t="s">
         <v>16</v>
       </c>
@@ -2438,7 +2487,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5">
       <c r="A68" t="s">
         <v>16</v>
       </c>
@@ -2455,7 +2504,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5">
       <c r="A69" t="s">
         <v>16</v>
       </c>
@@ -2472,7 +2521,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5">
       <c r="A70" t="s">
         <v>16</v>
       </c>
@@ -2489,7 +2538,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5">
       <c r="A71" t="s">
         <v>16</v>
       </c>
@@ -2506,7 +2555,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5">
       <c r="A72" t="s">
         <v>16</v>
       </c>
@@ -2523,7 +2572,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5">
       <c r="A73" t="s">
         <v>16</v>
       </c>
@@ -2540,7 +2589,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5">
       <c r="A74" t="s">
         <v>16</v>
       </c>
@@ -2557,7 +2606,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5">
       <c r="A75" t="s">
         <v>16</v>
       </c>
@@ -2574,7 +2623,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5">
       <c r="A76" t="s">
         <v>16</v>
       </c>
@@ -2591,7 +2640,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5">
       <c r="A77" t="s">
         <v>16</v>
       </c>
@@ -2608,7 +2657,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5">
       <c r="A78" t="s">
         <v>16</v>
       </c>
@@ -2625,7 +2674,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5">
       <c r="A79" t="s">
         <v>16</v>
       </c>
@@ -2642,7 +2691,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5">
       <c r="A80" t="s">
         <v>16</v>
       </c>
@@ -2659,7 +2708,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5">
       <c r="A81" t="s">
         <v>16</v>
       </c>
@@ -2676,7 +2725,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5">
       <c r="A82" t="s">
         <v>16</v>
       </c>
@@ -2693,7 +2742,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5">
       <c r="A83" t="s">
         <v>16</v>
       </c>
@@ -2710,7 +2759,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5">
       <c r="A84" t="s">
         <v>16</v>
       </c>
@@ -2727,7 +2776,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5">
       <c r="A85" t="s">
         <v>16</v>
       </c>
@@ -2744,7 +2793,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5">
       <c r="A86" t="s">
         <v>16</v>
       </c>
@@ -2761,7 +2810,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5">
       <c r="A87" t="s">
         <v>16</v>
       </c>
@@ -2778,7 +2827,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5">
       <c r="A88" t="s">
         <v>16</v>
       </c>
@@ -2795,7 +2844,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5">
       <c r="A89" t="s">
         <v>16</v>
       </c>
@@ -2812,7 +2861,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5">
       <c r="A90" t="s">
         <v>16</v>
       </c>
@@ -2829,7 +2878,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5">
       <c r="A91" t="s">
         <v>16</v>
       </c>
@@ -2846,7 +2895,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5">
       <c r="A92" t="s">
         <v>16</v>
       </c>
@@ -2863,7 +2912,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5">
       <c r="A93" t="s">
         <v>16</v>
       </c>
@@ -2880,7 +2929,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5">
       <c r="A94" t="s">
         <v>16</v>
       </c>
@@ -2897,7 +2946,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5">
       <c r="A95" t="s">
         <v>16</v>
       </c>
@@ -2914,7 +2963,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5">
       <c r="A96" t="s">
         <v>16</v>
       </c>
@@ -2931,7 +2980,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5">
       <c r="A97" t="s">
         <v>16</v>
       </c>
@@ -2948,7 +2997,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5">
       <c r="A98" t="s">
         <v>16</v>
       </c>
@@ -2965,7 +3014,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5">
       <c r="A99" t="s">
         <v>16</v>
       </c>
@@ -2982,7 +3031,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5">
       <c r="A100" t="s">
         <v>16</v>
       </c>
@@ -2999,7 +3048,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5">
       <c r="A101" t="s">
         <v>16</v>
       </c>
@@ -3016,7 +3065,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5">
       <c r="A102" t="s">
         <v>16</v>
       </c>
@@ -3033,7 +3082,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5">
       <c r="A103" t="s">
         <v>16</v>
       </c>
@@ -3050,7 +3099,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5">
       <c r="A104" t="s">
         <v>16</v>
       </c>
@@ -3067,7 +3116,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5">
       <c r="A105" t="s">
         <v>16</v>
       </c>
@@ -3084,7 +3133,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5">
       <c r="A106" t="s">
         <v>16</v>
       </c>
@@ -3101,7 +3150,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5">
       <c r="A107" t="s">
         <v>16</v>
       </c>
@@ -3118,7 +3167,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5">
       <c r="A108" t="s">
         <v>16</v>
       </c>
@@ -3135,7 +3184,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5">
       <c r="A109" t="s">
         <v>16</v>
       </c>
@@ -3152,7 +3201,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5">
       <c r="A110" t="s">
         <v>16</v>
       </c>
@@ -3169,7 +3218,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5">
       <c r="A111" t="s">
         <v>16</v>
       </c>
@@ -3186,7 +3235,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5">
       <c r="A112" t="s">
         <v>16</v>
       </c>
@@ -3203,7 +3252,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5">
       <c r="A113" t="s">
         <v>16</v>
       </c>
@@ -3220,7 +3269,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5">
       <c r="A114" t="s">
         <v>16</v>
       </c>
@@ -3237,7 +3286,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5">
       <c r="A115" t="s">
         <v>16</v>
       </c>
@@ -3254,7 +3303,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5">
       <c r="A116" t="s">
         <v>16</v>
       </c>
@@ -3271,7 +3320,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5">
       <c r="A117" t="s">
         <v>16</v>
       </c>
@@ -3288,7 +3337,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5">
       <c r="A118" t="s">
         <v>16</v>
       </c>
@@ -3305,7 +3354,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5">
       <c r="A119" t="s">
         <v>16</v>
       </c>
@@ -3322,7 +3371,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5">
       <c r="A120" t="s">
         <v>16</v>
       </c>
@@ -3339,7 +3388,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5">
       <c r="A121" t="s">
         <v>16</v>
       </c>
@@ -3356,7 +3405,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5">
       <c r="A122" t="s">
         <v>16</v>
       </c>
@@ -3373,7 +3422,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5">
       <c r="A123" t="s">
         <v>16</v>
       </c>
@@ -3390,7 +3439,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5">
       <c r="A124" t="s">
         <v>16</v>
       </c>
@@ -3407,7 +3456,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5">
       <c r="A125" t="s">
         <v>16</v>
       </c>
@@ -3424,7 +3473,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5">
       <c r="A126" t="s">
         <v>16</v>
       </c>
@@ -3441,7 +3490,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5">
       <c r="A127" t="s">
         <v>16</v>
       </c>
@@ -3458,7 +3507,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5">
       <c r="A128" t="s">
         <v>16</v>
       </c>
@@ -3475,7 +3524,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5">
       <c r="A129" t="s">
         <v>16</v>
       </c>
@@ -3492,7 +3541,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5">
       <c r="A130" t="s">
         <v>16</v>
       </c>
@@ -3509,7 +3558,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5">
       <c r="A131" t="s">
         <v>16</v>
       </c>
@@ -3526,7 +3575,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5">
       <c r="A132" t="s">
         <v>16</v>
       </c>
@@ -3543,7 +3592,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5">
       <c r="A133" t="s">
         <v>16</v>
       </c>
@@ -3560,7 +3609,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5">
       <c r="A134" t="s">
         <v>16</v>
       </c>
@@ -3577,7 +3626,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5">
       <c r="A135" t="s">
         <v>16</v>
       </c>
@@ -3594,7 +3643,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5">
       <c r="A136" t="s">
         <v>16</v>
       </c>
@@ -3611,7 +3660,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5">
       <c r="A137" t="s">
         <v>16</v>
       </c>
@@ -3628,7 +3677,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5">
       <c r="A138" t="s">
         <v>16</v>
       </c>
@@ -3645,7 +3694,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5">
       <c r="A139" t="s">
         <v>16</v>
       </c>
@@ -3662,7 +3711,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5">
       <c r="A140" t="s">
         <v>16</v>
       </c>
@@ -3679,7 +3728,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5">
       <c r="A141" t="s">
         <v>16</v>
       </c>
@@ -3696,7 +3745,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5">
       <c r="A142" t="s">
         <v>16</v>
       </c>
@@ -3713,7 +3762,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5">
       <c r="A143" t="s">
         <v>16</v>
       </c>
@@ -3730,7 +3779,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5">
       <c r="A144" t="s">
         <v>16</v>
       </c>
@@ -3747,7 +3796,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5">
       <c r="A145" t="s">
         <v>16</v>
       </c>
@@ -3764,7 +3813,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5">
       <c r="A146" t="s">
         <v>16</v>
       </c>
@@ -3781,7 +3830,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5">
       <c r="A147" t="s">
         <v>16</v>
       </c>
@@ -3798,7 +3847,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5">
       <c r="A148" t="s">
         <v>16</v>
       </c>
@@ -3815,7 +3864,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5">
       <c r="A149" t="s">
         <v>16</v>
       </c>
@@ -3832,7 +3881,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5">
       <c r="A150" t="s">
         <v>16</v>
       </c>
@@ -3849,7 +3898,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5">
       <c r="A151" t="s">
         <v>16</v>
       </c>
@@ -3866,7 +3915,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5">
       <c r="A152" t="s">
         <v>16</v>
       </c>
@@ -3883,7 +3932,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5">
       <c r="A153" t="s">
         <v>16</v>
       </c>
@@ -3900,7 +3949,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5">
       <c r="A154" t="s">
         <v>16</v>
       </c>
@@ -3917,7 +3966,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5">
       <c r="A155" t="s">
         <v>16</v>
       </c>
@@ -3934,7 +3983,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5">
       <c r="A156" t="s">
         <v>16</v>
       </c>
@@ -3951,7 +4000,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5">
       <c r="A157" t="s">
         <v>16</v>
       </c>
@@ -3968,7 +4017,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5">
       <c r="A158" t="s">
         <v>16</v>
       </c>
@@ -3985,7 +4034,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5">
       <c r="A159" t="s">
         <v>16</v>
       </c>
@@ -4002,7 +4051,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5">
       <c r="A160" t="s">
         <v>16</v>
       </c>
@@ -4019,7 +4068,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5">
       <c r="A161" t="s">
         <v>16</v>
       </c>
@@ -4036,7 +4085,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5">
       <c r="A162" t="s">
         <v>16</v>
       </c>
@@ -4053,7 +4102,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5">
       <c r="A163" t="s">
         <v>16</v>
       </c>
@@ -4070,7 +4119,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5">
       <c r="A164" t="s">
         <v>16</v>
       </c>
@@ -4087,7 +4136,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5">
       <c r="A165" t="s">
         <v>16</v>
       </c>
@@ -4104,7 +4153,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5">
       <c r="A166" t="s">
         <v>16</v>
       </c>
@@ -4121,7 +4170,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5">
       <c r="A167" t="s">
         <v>16</v>
       </c>
@@ -4138,7 +4187,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5">
       <c r="A168" t="s">
         <v>16</v>
       </c>
@@ -4155,7 +4204,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5">
       <c r="A169" t="s">
         <v>16</v>
       </c>
@@ -4172,7 +4221,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5">
       <c r="A170" t="s">
         <v>16</v>
       </c>
@@ -4189,7 +4238,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5">
       <c r="A171" t="s">
         <v>16</v>
       </c>
@@ -4206,7 +4255,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5">
       <c r="A172" t="s">
         <v>16</v>
       </c>
@@ -4223,7 +4272,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5">
       <c r="A173" t="s">
         <v>16</v>
       </c>
@@ -4240,7 +4289,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5">
       <c r="A174" t="s">
         <v>16</v>
       </c>
@@ -4257,7 +4306,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5">
       <c r="A175" t="s">
         <v>16</v>
       </c>
@@ -4274,7 +4323,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5">
       <c r="A176" t="s">
         <v>16</v>
       </c>
@@ -4291,7 +4340,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5">
       <c r="A177" t="s">
         <v>16</v>
       </c>
@@ -4308,7 +4357,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5">
       <c r="A178" t="s">
         <v>16</v>
       </c>
@@ -4325,7 +4374,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5">
       <c r="A179" t="s">
         <v>16</v>
       </c>
@@ -4342,7 +4391,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5">
       <c r="A180" t="s">
         <v>16</v>
       </c>
@@ -4359,7 +4408,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5">
       <c r="A181" t="s">
         <v>16</v>
       </c>
@@ -4376,7 +4425,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5">
       <c r="A182" t="s">
         <v>16</v>
       </c>
@@ -4393,7 +4442,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5">
       <c r="A183" t="s">
         <v>16</v>
       </c>
@@ -4410,7 +4459,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5">
       <c r="A184" t="s">
         <v>16</v>
       </c>
@@ -4427,7 +4476,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5">
       <c r="A185" t="s">
         <v>16</v>
       </c>
@@ -4444,7 +4493,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5">
       <c r="A186" t="s">
         <v>16</v>
       </c>
@@ -4461,7 +4510,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:5">
       <c r="A187" t="s">
         <v>16</v>
       </c>
@@ -4478,7 +4527,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:5">
       <c r="A188" t="s">
         <v>16</v>
       </c>
@@ -4495,7 +4544,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:5">
       <c r="A189" t="s">
         <v>16</v>
       </c>
@@ -4512,7 +4561,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:5">
       <c r="A190" t="s">
         <v>16</v>
       </c>
@@ -4529,7 +4578,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:5">
       <c r="A191" t="s">
         <v>16</v>
       </c>
@@ -4546,7 +4595,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:5">
       <c r="A192" t="s">
         <v>16</v>
       </c>
@@ -4563,7 +4612,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:5">
       <c r="A193" t="s">
         <v>16</v>
       </c>
@@ -4580,7 +4629,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5">
       <c r="A194" t="s">
         <v>16</v>
       </c>
@@ -4597,7 +4646,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:5">
       <c r="A195" t="s">
         <v>16</v>
       </c>
@@ -4614,7 +4663,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:5">
       <c r="A196" t="s">
         <v>16</v>
       </c>
@@ -4631,7 +4680,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:5">
       <c r="A197" t="s">
         <v>16</v>
       </c>
@@ -4648,7 +4697,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5">
       <c r="A198" t="s">
         <v>16</v>
       </c>
@@ -4665,7 +4714,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:5">
       <c r="A199" t="s">
         <v>16</v>
       </c>
@@ -4682,7 +4731,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:5">
       <c r="A200" t="s">
         <v>16</v>
       </c>
@@ -4699,7 +4748,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:5">
       <c r="A201" t="s">
         <v>16</v>
       </c>
@@ -4716,7 +4765,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:5">
       <c r="A202" t="s">
         <v>16</v>
       </c>
@@ -4733,7 +4782,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:5">
       <c r="A203" t="s">
         <v>16</v>
       </c>
@@ -4750,7 +4799,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:5">
       <c r="A204" t="s">
         <v>16</v>
       </c>
@@ -4767,7 +4816,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:5">
       <c r="A205" t="s">
         <v>16</v>
       </c>
@@ -4784,7 +4833,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:5">
       <c r="A206" t="s">
         <v>16</v>
       </c>
@@ -4801,7 +4850,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:5">
       <c r="A207" t="s">
         <v>16</v>
       </c>
@@ -4818,7 +4867,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:5">
       <c r="A208" t="s">
         <v>16</v>
       </c>
@@ -4835,7 +4884,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:5">
       <c r="A209" t="s">
         <v>16</v>
       </c>
@@ -4852,7 +4901,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:5">
       <c r="A210" t="s">
         <v>16</v>
       </c>
@@ -4869,7 +4918,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:5">
       <c r="A211" t="s">
         <v>16</v>
       </c>
@@ -4886,7 +4935,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:5">
       <c r="A212" t="s">
         <v>16</v>
       </c>
@@ -4903,7 +4952,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:5">
       <c r="A213" t="s">
         <v>16</v>
       </c>
@@ -4920,7 +4969,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:5">
       <c r="A214" t="s">
         <v>16</v>
       </c>
@@ -4937,7 +4986,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:5">
       <c r="A215" t="s">
         <v>16</v>
       </c>
@@ -4954,7 +5003,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:5">
       <c r="A216" t="s">
         <v>16</v>
       </c>
@@ -4971,7 +5020,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:5">
       <c r="A217" t="s">
         <v>16</v>
       </c>
@@ -4988,7 +5037,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:5">
       <c r="A218" t="s">
         <v>16</v>
       </c>
@@ -5005,7 +5054,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:5">
       <c r="A219" t="s">
         <v>16</v>
       </c>
@@ -5022,7 +5071,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:5">
       <c r="A220" t="s">
         <v>16</v>
       </c>
@@ -5039,7 +5088,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:5">
       <c r="A221" t="s">
         <v>16</v>
       </c>
@@ -5056,7 +5105,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:5">
       <c r="A222" t="s">
         <v>16</v>
       </c>
@@ -5073,7 +5122,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:5">
       <c r="A223" t="s">
         <v>16</v>
       </c>
@@ -5090,7 +5139,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:5">
       <c r="A224" t="s">
         <v>16</v>
       </c>
@@ -5107,7 +5156,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:5">
       <c r="A225" t="s">
         <v>16</v>
       </c>
@@ -5124,7 +5173,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:5">
       <c r="A226" t="s">
         <v>16</v>
       </c>
@@ -5141,7 +5190,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:5">
       <c r="A227" t="s">
         <v>16</v>
       </c>
@@ -5158,7 +5207,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:5">
       <c r="A228" t="s">
         <v>16</v>
       </c>
@@ -5175,7 +5224,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:5">
       <c r="A229" t="s">
         <v>16</v>
       </c>
@@ -5192,7 +5241,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:5">
       <c r="A230" t="s">
         <v>16</v>
       </c>
@@ -5209,7 +5258,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:5">
       <c r="A231" t="s">
         <v>16</v>
       </c>
@@ -5226,7 +5275,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:5">
       <c r="A232" t="s">
         <v>16</v>
       </c>
@@ -5243,7 +5292,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:5">
       <c r="A233" t="s">
         <v>16</v>
       </c>
@@ -5260,7 +5309,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:5">
       <c r="A234" t="s">
         <v>16</v>
       </c>
@@ -5277,7 +5326,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:5">
       <c r="A235" t="s">
         <v>16</v>
       </c>
@@ -5294,7 +5343,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:5">
       <c r="A236" t="s">
         <v>16</v>
       </c>
@@ -5311,7 +5360,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:5">
       <c r="A237" t="s">
         <v>16</v>
       </c>
@@ -5328,7 +5377,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:5">
       <c r="A238" t="s">
         <v>16</v>
       </c>
@@ -5345,7 +5394,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:5">
       <c r="A239" t="s">
         <v>16</v>
       </c>
@@ -5362,7 +5411,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:5">
       <c r="A240" t="s">
         <v>16</v>
       </c>
@@ -5379,7 +5428,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:5">
       <c r="A241" t="s">
         <v>16</v>
       </c>
@@ -5396,7 +5445,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:5">
       <c r="A242" t="s">
         <v>16</v>
       </c>
@@ -5413,7 +5462,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:5">
       <c r="A243" t="s">
         <v>16</v>
       </c>
@@ -5430,7 +5479,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:5">
       <c r="A244" t="s">
         <v>16</v>
       </c>
@@ -5447,7 +5496,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:5">
       <c r="A245" t="s">
         <v>16</v>
       </c>
@@ -5464,7 +5513,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:5">
       <c r="A246" t="s">
         <v>16</v>
       </c>
@@ -5481,7 +5530,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:5">
       <c r="A247" t="s">
         <v>16</v>
       </c>
@@ -5498,7 +5547,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:5">
       <c r="A248" t="s">
         <v>16</v>
       </c>
@@ -5515,7 +5564,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:5">
       <c r="A249" t="s">
         <v>16</v>
       </c>
@@ -5532,7 +5581,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:5">
       <c r="A250" t="s">
         <v>16</v>
       </c>
@@ -5549,7 +5598,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:5">
       <c r="A251" t="s">
         <v>16</v>
       </c>
@@ -5566,7 +5615,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:5">
       <c r="A252" t="s">
         <v>16</v>
       </c>
@@ -5583,7 +5632,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:5">
       <c r="A253" t="s">
         <v>16</v>
       </c>
@@ -5600,7 +5649,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:5">
       <c r="A254" t="s">
         <v>16</v>
       </c>
@@ -5617,7 +5666,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:5">
       <c r="A255" t="s">
         <v>16</v>
       </c>
@@ -5634,7 +5683,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:5">
       <c r="A256" t="s">
         <v>16</v>
       </c>
@@ -5651,7 +5700,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:5">
       <c r="A257" t="s">
         <v>16</v>
       </c>
@@ -5668,7 +5717,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:5">
       <c r="A258" t="s">
         <v>16</v>
       </c>
@@ -5685,7 +5734,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:5">
       <c r="A259" t="s">
         <v>16</v>
       </c>
@@ -5702,7 +5751,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:5">
       <c r="A260" t="s">
         <v>16</v>
       </c>
@@ -5719,7 +5768,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:5">
       <c r="A261" t="s">
         <v>16</v>
       </c>
@@ -5736,7 +5785,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:5">
       <c r="A262" t="s">
         <v>16</v>
       </c>
@@ -5753,7 +5802,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:5">
       <c r="A263" t="s">
         <v>16</v>
       </c>
@@ -5770,7 +5819,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:5">
       <c r="A264" t="s">
         <v>16</v>
       </c>
@@ -5787,7 +5836,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:5">
       <c r="A265" t="s">
         <v>16</v>
       </c>
@@ -5804,7 +5853,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:5">
       <c r="A266" t="s">
         <v>16</v>
       </c>
@@ -5821,7 +5870,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:5">
       <c r="A267" t="s">
         <v>16</v>
       </c>
@@ -5838,7 +5887,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:5">
       <c r="A268" t="s">
         <v>16</v>
       </c>
@@ -5855,7 +5904,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:5">
       <c r="A269" t="s">
         <v>16</v>
       </c>
@@ -5872,7 +5921,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:5">
       <c r="A270" t="s">
         <v>16</v>
       </c>
@@ -5889,7 +5938,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:5">
       <c r="A271" t="s">
         <v>16</v>
       </c>
@@ -5906,7 +5955,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:5">
       <c r="A272" t="s">
         <v>16</v>
       </c>
@@ -5923,7 +5972,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:5">
       <c r="A273" t="s">
         <v>16</v>
       </c>
@@ -5940,7 +5989,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:5">
       <c r="A274" t="s">
         <v>16</v>
       </c>
@@ -5957,7 +6006,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:5">
       <c r="A275" t="s">
         <v>16</v>
       </c>
@@ -5974,7 +6023,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:5">
       <c r="A276" t="s">
         <v>16</v>
       </c>
@@ -5991,7 +6040,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:5">
       <c r="A277" t="s">
         <v>16</v>
       </c>
@@ -6008,7 +6057,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:5">
       <c r="A278" t="s">
         <v>16</v>
       </c>
@@ -6025,7 +6074,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:5">
       <c r="A279" t="s">
         <v>16</v>
       </c>
@@ -6042,7 +6091,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:5">
       <c r="A280" t="s">
         <v>16</v>
       </c>
@@ -6059,7 +6108,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:5">
       <c r="A281" t="s">
         <v>16</v>
       </c>
@@ -6076,7 +6125,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:5">
       <c r="A282" t="s">
         <v>16</v>
       </c>
@@ -6093,7 +6142,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:5">
       <c r="A283" t="s">
         <v>16</v>
       </c>
@@ -6110,7 +6159,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:5">
       <c r="A284" t="s">
         <v>16</v>
       </c>
@@ -6127,7 +6176,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:5">
       <c r="A285" t="s">
         <v>16</v>
       </c>
@@ -6144,7 +6193,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:5">
       <c r="A286" t="s">
         <v>16</v>
       </c>
@@ -6161,7 +6210,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:5">
       <c r="A287" t="s">
         <v>16</v>
       </c>
@@ -6178,7 +6227,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:5">
       <c r="A288" t="s">
         <v>16</v>
       </c>
@@ -6195,7 +6244,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:5">
       <c r="A289" t="s">
         <v>16</v>
       </c>
@@ -6212,7 +6261,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:5">
       <c r="A290" t="s">
         <v>16</v>
       </c>
@@ -6229,7 +6278,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:5">
       <c r="A291" t="s">
         <v>16</v>
       </c>
@@ -6246,7 +6295,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:5">
       <c r="A292" t="s">
         <v>16</v>
       </c>
@@ -6263,7 +6312,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:5">
       <c r="A293" t="s">
         <v>16</v>
       </c>
@@ -6280,7 +6329,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:5">
       <c r="A294" t="s">
         <v>16</v>
       </c>
@@ -6297,7 +6346,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:5">
       <c r="A295" t="s">
         <v>16</v>
       </c>
@@ -6314,7 +6363,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:5">
       <c r="A296" t="s">
         <v>16</v>
       </c>
@@ -6331,7 +6380,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:5">
       <c r="A297" t="s">
         <v>16</v>
       </c>
@@ -6348,7 +6397,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:5">
       <c r="A298" t="s">
         <v>16</v>
       </c>
@@ -6365,7 +6414,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:5">
       <c r="A299" t="s">
         <v>16</v>
       </c>
@@ -6382,7 +6431,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:5">
       <c r="A300" t="s">
         <v>16</v>
       </c>
@@ -6399,7 +6448,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:5">
       <c r="A301" t="s">
         <v>16</v>
       </c>
@@ -6416,7 +6465,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="302" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:5">
       <c r="A302" t="s">
         <v>16</v>
       </c>
@@ -6433,7 +6482,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="303" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:5">
       <c r="A303" t="s">
         <v>16</v>
       </c>
@@ -6450,7 +6499,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="304" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:5">
       <c r="A304" t="s">
         <v>16</v>
       </c>
@@ -6467,7 +6516,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="305" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:5">
       <c r="A305" t="s">
         <v>16</v>
       </c>
@@ -6484,7 +6533,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="306" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:5">
       <c r="A306" t="s">
         <v>16</v>
       </c>
@@ -6501,7 +6550,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="307" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:5">
       <c r="A307" t="s">
         <v>16</v>
       </c>
@@ -6518,7 +6567,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="308" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:5">
       <c r="A308" t="s">
         <v>16</v>
       </c>
@@ -6535,7 +6584,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="309" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:5">
       <c r="A309" t="s">
         <v>16</v>
       </c>
@@ -6552,7 +6601,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="310" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:5">
       <c r="A310" t="s">
         <v>16</v>
       </c>
@@ -6569,7 +6618,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="311" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:5">
       <c r="A311" t="s">
         <v>16</v>
       </c>
@@ -6586,7 +6635,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="312" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:5">
       <c r="A312" t="s">
         <v>16</v>
       </c>
@@ -6603,7 +6652,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="313" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:5">
       <c r="A313" t="s">
         <v>16</v>
       </c>
@@ -6620,7 +6669,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="314" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:5">
       <c r="A314" t="s">
         <v>16</v>
       </c>
@@ -6637,7 +6686,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="315" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:5">
       <c r="A315" t="s">
         <v>16</v>
       </c>
@@ -6654,7 +6703,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="316" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:5">
       <c r="A316" t="s">
         <v>16</v>
       </c>
@@ -6671,7 +6720,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="317" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:5">
       <c r="A317" t="s">
         <v>16</v>
       </c>
@@ -6688,7 +6737,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="318" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:5">
       <c r="A318" t="s">
         <v>16</v>
       </c>
@@ -6705,7 +6754,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="319" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:5">
       <c r="A319" t="s">
         <v>16</v>
       </c>
@@ -6722,7 +6771,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="320" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:5">
       <c r="A320" t="s">
         <v>16</v>
       </c>
@@ -6739,7 +6788,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="321" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:5">
       <c r="A321" t="s">
         <v>16</v>
       </c>
@@ -6756,31 +6805,340 @@
         <v>15</v>
       </c>
     </row>
+    <row r="322" spans="1:5">
+      <c r="A322" t="s">
+        <v>16</v>
+      </c>
+      <c r="B322">
+        <v>58</v>
+      </c>
+      <c r="C322" t="s">
+        <v>17</v>
+      </c>
+      <c r="D322" t="s">
+        <v>312</v>
+      </c>
+      <c r="E322" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="323" spans="1:5">
+      <c r="A323" t="s">
+        <v>16</v>
+      </c>
+      <c r="B323">
+        <v>58</v>
+      </c>
+      <c r="C323" t="s">
+        <v>17</v>
+      </c>
+      <c r="D323" t="s">
+        <v>313</v>
+      </c>
+      <c r="E323" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="324" spans="1:5">
+      <c r="A324" t="s">
+        <v>16</v>
+      </c>
+      <c r="B324">
+        <v>58</v>
+      </c>
+      <c r="C324" t="s">
+        <v>17</v>
+      </c>
+      <c r="D324" t="s">
+        <v>314</v>
+      </c>
+      <c r="E324" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="325" spans="1:5">
+      <c r="A325" t="s">
+        <v>16</v>
+      </c>
+      <c r="B325">
+        <v>58</v>
+      </c>
+      <c r="C325" t="s">
+        <v>17</v>
+      </c>
+      <c r="D325" t="s">
+        <v>315</v>
+      </c>
+      <c r="E325" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="326" spans="1:5">
+      <c r="A326" t="s">
+        <v>16</v>
+      </c>
+      <c r="B326">
+        <v>58</v>
+      </c>
+      <c r="C326" t="s">
+        <v>17</v>
+      </c>
+      <c r="D326" t="s">
+        <v>316</v>
+      </c>
+      <c r="E326" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="327" spans="1:5">
+      <c r="A327" t="s">
+        <v>16</v>
+      </c>
+      <c r="B327">
+        <v>58</v>
+      </c>
+      <c r="C327" t="s">
+        <v>17</v>
+      </c>
+      <c r="D327" t="s">
+        <v>317</v>
+      </c>
+      <c r="E327" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="328" spans="1:5">
+      <c r="A328" t="s">
+        <v>16</v>
+      </c>
+      <c r="B328">
+        <v>58</v>
+      </c>
+      <c r="C328" t="s">
+        <v>17</v>
+      </c>
+      <c r="D328" t="s">
+        <v>318</v>
+      </c>
+      <c r="E328" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="329" spans="1:5">
+      <c r="A329" t="s">
+        <v>16</v>
+      </c>
+      <c r="B329">
+        <v>58</v>
+      </c>
+      <c r="C329" t="s">
+        <v>17</v>
+      </c>
+      <c r="D329" t="s">
+        <v>319</v>
+      </c>
+      <c r="E329" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="330" spans="1:5">
+      <c r="A330" t="s">
+        <v>16</v>
+      </c>
+      <c r="B330">
+        <v>58</v>
+      </c>
+      <c r="C330" t="s">
+        <v>17</v>
+      </c>
+      <c r="D330" t="s">
+        <v>320</v>
+      </c>
+      <c r="E330" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="331" spans="1:5">
+      <c r="A331" t="s">
+        <v>16</v>
+      </c>
+      <c r="B331">
+        <v>58</v>
+      </c>
+      <c r="C331" t="s">
+        <v>17</v>
+      </c>
+      <c r="D331" t="s">
+        <v>321</v>
+      </c>
+      <c r="E331" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="332" spans="1:5">
+      <c r="A332" t="s">
+        <v>16</v>
+      </c>
+      <c r="B332">
+        <v>58</v>
+      </c>
+      <c r="C332" t="s">
+        <v>17</v>
+      </c>
+      <c r="D332" t="s">
+        <v>322</v>
+      </c>
+      <c r="E332" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="333" spans="1:5">
+      <c r="A333" t="s">
+        <v>16</v>
+      </c>
+      <c r="B333">
+        <v>58</v>
+      </c>
+      <c r="C333" t="s">
+        <v>17</v>
+      </c>
+      <c r="D333" t="s">
+        <v>323</v>
+      </c>
+      <c r="E333" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="334" spans="1:5">
+      <c r="A334" t="s">
+        <v>16</v>
+      </c>
+      <c r="B334">
+        <v>58</v>
+      </c>
+      <c r="C334" t="s">
+        <v>17</v>
+      </c>
+      <c r="D334" t="s">
+        <v>324</v>
+      </c>
+      <c r="E334" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="335" spans="1:5">
+      <c r="A335" t="s">
+        <v>16</v>
+      </c>
+      <c r="B335">
+        <v>58</v>
+      </c>
+      <c r="C335" t="s">
+        <v>17</v>
+      </c>
+      <c r="D335" t="s">
+        <v>325</v>
+      </c>
+      <c r="E335" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="336" spans="1:5">
+      <c r="A336" t="s">
+        <v>16</v>
+      </c>
+      <c r="B336">
+        <v>58</v>
+      </c>
+      <c r="C336" t="s">
+        <v>17</v>
+      </c>
+      <c r="D336" t="s">
+        <v>326</v>
+      </c>
+      <c r="E336" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="337" spans="1:5">
+      <c r="A337" t="s">
+        <v>16</v>
+      </c>
+      <c r="B337">
+        <v>58</v>
+      </c>
+      <c r="C337" t="s">
+        <v>17</v>
+      </c>
+      <c r="D337" t="s">
+        <v>327</v>
+      </c>
+      <c r="E337" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="338" spans="1:5">
+      <c r="A338" t="s">
+        <v>16</v>
+      </c>
+      <c r="B338">
+        <v>58</v>
+      </c>
+      <c r="C338" t="s">
+        <v>17</v>
+      </c>
+      <c r="D338" t="s">
+        <v>328</v>
+      </c>
+      <c r="E338" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="339" spans="1:5">
+      <c r="A339" t="s">
+        <v>16</v>
+      </c>
+      <c r="B339">
+        <v>58</v>
+      </c>
+      <c r="C339" t="s">
+        <v>17</v>
+      </c>
+      <c r="D339" t="s">
+        <v>329</v>
+      </c>
+      <c r="E339" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
+  <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
+  <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>